<commit_message>
Added SoftUni exam to MI Course
</commit_message>
<xml_diff>
--- a/II. Software Technologies & Design - Group 3A/STD 3A - results.xlsx
+++ b/II. Software Technologies & Design - Group 3A/STD 3A - results.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,7 +521,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>1601681079</v>
+        <v>1601681081</v>
       </c>
       <c r="C7">
         <v>5</v>

</xml_diff>